<commit_message>
Confirmed wheel analysis, added wheels to BOM
</commit_message>
<xml_diff>
--- a/Analysis/Mechanical Analysis.xlsx
+++ b/Analysis/Mechanical Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\Sid\Projects\Smart Cart\smart-cart\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tk7363\Desktop\smart-cart\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +769,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -815,7 +815,7 @@
       </c>
       <c r="E6" s="1">
         <f>A6*(A3/3)*A4</f>
-        <v>20.000000000000004</v>
+        <v>26.666666666666671</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
@@ -836,7 +836,7 @@
       </c>
       <c r="E7" s="1">
         <f>A3*A4*(SIN(RADIANS(A9)) + (A8/32.2))/(A20*A5)</f>
-        <v>2.0212140733376791</v>
+        <v>2.6949520977835721</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="E8" s="2">
         <f>E7*16</f>
-        <v>32.339425173402866</v>
+        <v>43.119233564537154</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -876,7 +876,7 @@
       </c>
       <c r="E9" s="1">
         <f>A7*12/A4</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -897,7 +897,7 @@
       </c>
       <c r="E10" s="2">
         <f>(E9/(2*PI()))*60</f>
-        <v>190.98593171027443</v>
+        <v>143.23944878270581</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
@@ -943,7 +943,7 @@
       </c>
       <c r="E15" s="1">
         <f>E8/(E14*A14)</f>
-        <v>39.151846456904195</v>
+        <v>52.202461942538932</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -964,7 +964,7 @@
       </c>
       <c r="E16" s="1">
         <f>E10*E14</f>
-        <v>225.36339941812381</v>
+        <v>169.02254956359283</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>13</v>
@@ -976,7 +976,7 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
         <f>(E15*0.0070615518333333)*(E16*0.104719755)</f>
-        <v>6.5247579103211795</v>
+        <v>6.5247579103211786</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>15</v>
@@ -986,7 +986,7 @@
       </c>
       <c r="J17" s="1">
         <f>E21*18.75*64/60</f>
-        <v>4508.5188618333686</v>
+        <v>3678.025149111159</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>70</v>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E20" s="1">
         <f>E15</f>
-        <v>39.151846456904195</v>
+        <v>52.202461942538932</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="E21" s="1">
         <f>(-350*E15/110) + 350</f>
-        <v>225.42594309166847</v>
+        <v>183.90125745555795</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>13</v>
@@ -1043,7 +1043,7 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
         <f>E21/E10</f>
-        <v>1.1803274779088939</v>
+        <v>1.2838729764629022</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>61</v>
@@ -1052,7 +1052,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
         <f>(E20*0.0070615518333333)*(E21*0.104719755)</f>
-        <v>6.5265686849622906</v>
+        <v>7.0991189483253549</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>15</v>
@@ -1064,7 +1064,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
         <f>E20*E14*A14</f>
-        <v>32.339425173402866</v>
+        <v>43.119233564537154</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -1076,7 +1076,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
         <f>E21/E14</f>
-        <v>191.03893482344787</v>
+        <v>155.848523267422</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>13</v>
@@ -1088,7 +1088,7 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <f>(E21/E14)*2*PI()*A4/(60*12)</f>
-        <v>5.0013876182580264</v>
+        <v>5.4401397307750097</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>7</v>
@@ -1100,7 +1100,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <f>E23/(A20*A10)</f>
-        <v>3.6258714916457175</v>
+        <v>1.9719774856459322</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>24</v>
@@ -1124,7 +1124,7 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>E20/(16*A15)</f>
-        <v>2.4469904035565122</v>
+        <v>3.2626538714086832</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="E31" s="1">
         <f>(A31*A32/(16*A33*A34))/1000</f>
-        <v>0.29363884842678145</v>
+        <v>0.39151846456904194</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>51</v>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="E32" s="1">
         <f>A35/E31</f>
-        <v>51.083159058704162</v>
+        <v>38.312369294028123</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>31</v>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="E33" s="1">
         <f>(A31*A32/(16*A36*A37))/1000</f>
-        <v>0.18352428026673839</v>
+        <v>0.24469904035565121</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>51</v>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="E34" s="1">
         <f>A38/E33</f>
-        <v>81.733054493926673</v>
+        <v>61.299790870444994</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>30</v>

</xml_diff>